<commit_message>
incorporated suggestion from Dr. Pickett
</commit_message>
<xml_diff>
--- a/geo_ncbi/geo_host_transcriptome.xlsx
+++ b/geo_ncbi/geo_host_transcriptome.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abquaye/MyStuff/host_rna_seq/geo_ncbi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED60CB-58F1-5E41-BEEA-2D91E6E25A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F91840-2182-9348-BE04-14B407A5225B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="qZzD4R9MHkY34uacjqt3UDyeD61BQpRgIo5GituA+M5TJZYrZGlKZCDSkAkMk0lzHa20F9kBcNHoSPrpZkW+dg==" workbookSaltValue="NTRFdVUfx51db2iwG+fWhA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="41120" windowHeight="25720" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="860" windowWidth="28740" windowHeight="25720" tabRatio="874" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="4" r:id="rId1"/>
@@ -815,23 +815,249 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Format:  Firstname, Initial, Lastname
-Example:  Jane, Doe
-Example:  Yixin, Wang
-Example:  John, H, Smith
-Example:  Charles,E,Determan Jr
-Example:  Monique,G,van der Wijst
-Example:  Mark, Anderson Dumont
-Each contributor on a separate line.
-Add as many contributor lines as needed.</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Format:  Firstname, Initial, Lastname
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Jane, Doe
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Yixin, Wang
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  John, H, Smith
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Charles,E,Determan Jr
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Monique,G,van der Wijst
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Mark, Anderson Dumont
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Each contributor on a separate line.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Add as many contributor lines as needed.</t>
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{F6E95742-D022-4834-BCC4-6983612D842F}">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{0F576F69-8602-744E-B4DB-2D3F9EF04838}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Format:  Firstname, Initial, Lastname
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Jane, Doe
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Yixin, Wang
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  John, H, Smith
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Charles,E,Determan Jr
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Monique,G,van der Wijst
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Example:  Mark, Anderson Dumont
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Each contributor on a separate line.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Add as many contributor lines as needed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="0" shapeId="0" xr:uid="{F6E95742-D022-4834-BCC4-6983612D842F}">
       <text>
         <r>
           <rPr>
@@ -856,7 +1082,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{CF8D5531-D910-4421-AA94-945F769233A4}">
+    <comment ref="B38" authorId="0" shapeId="0" xr:uid="{CF8D5531-D910-4421-AA94-945F769233A4}">
       <text>
         <r>
           <rPr>
@@ -935,7 +1161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C37" authorId="1" shapeId="0" xr:uid="{9C70704D-0D4F-457F-B72D-A68E84A94DB8}">
+    <comment ref="C38" authorId="1" shapeId="0" xr:uid="{9C70704D-0D4F-457F-B72D-A68E84A94DB8}">
       <text>
         <r>
           <rPr>
@@ -950,7 +1176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D37" authorId="0" shapeId="0" xr:uid="{CFA00CB9-BDA3-4049-9D2D-A6EDD4CAB2F7}">
+    <comment ref="D38" authorId="0" shapeId="0" xr:uid="{CFA00CB9-BDA3-4049-9D2D-A6EDD4CAB2F7}">
       <text>
         <r>
           <rPr>
@@ -1118,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E37" authorId="0" shapeId="0" xr:uid="{8AE2DED2-1910-46DD-B003-E3B926CF13F9}">
+    <comment ref="E38" authorId="0" shapeId="0" xr:uid="{8AE2DED2-1910-46DD-B003-E3B926CF13F9}">
       <text>
         <r>
           <rPr>
@@ -1286,7 +1512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{FFA9B3EE-9B03-459B-86E5-04A915F98CD6}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{FFA9B3EE-9B03-459B-86E5-04A915F98CD6}">
       <text>
         <r>
           <rPr>
@@ -1314,7 +1540,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G37" authorId="0" shapeId="0" xr:uid="{DC9A309F-98B6-47F7-89F3-640B59ACA3A2}">
+    <comment ref="G38" authorId="0" shapeId="0" xr:uid="{DC9A309F-98B6-47F7-89F3-640B59ACA3A2}">
       <text>
         <r>
           <rPr>
@@ -1482,7 +1708,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H37" authorId="0" shapeId="0" xr:uid="{F237F1AC-2F04-47B1-AB58-5490E2A3D37F}">
+    <comment ref="H38" authorId="0" shapeId="0" xr:uid="{F237F1AC-2F04-47B1-AB58-5490E2A3D37F}">
       <text>
         <r>
           <rPr>
@@ -1650,7 +1876,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I37" authorId="0" shapeId="0" xr:uid="{2B95163B-4F70-4260-8B3E-FA5E66C3FA34}">
+    <comment ref="I38" authorId="0" shapeId="0" xr:uid="{2B95163B-4F70-4260-8B3E-FA5E66C3FA34}">
       <text>
         <r>
           <rPr>
@@ -1763,7 +1989,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J37" authorId="0" shapeId="0" xr:uid="{08FCF47F-A4B9-46CE-B5C2-AD8BF8BBD639}">
+    <comment ref="J38" authorId="0" shapeId="0" xr:uid="{08FCF47F-A4B9-46CE-B5C2-AD8BF8BBD639}">
       <text>
         <r>
           <rPr>
@@ -1777,7 +2003,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K37" authorId="0" shapeId="0" xr:uid="{D77C088E-1F65-434F-91C8-6FAEA5F6C04F}">
+    <comment ref="K38" authorId="0" shapeId="0" xr:uid="{D77C088E-1F65-434F-91C8-6FAEA5F6C04F}">
       <text>
         <r>
           <rPr>
@@ -2427,7 +2653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L37" authorId="0" shapeId="0" xr:uid="{4B13B8A9-64B8-480C-ACA7-17CF82E46745}">
+    <comment ref="L38" authorId="0" shapeId="0" xr:uid="{4B13B8A9-64B8-480C-ACA7-17CF82E46745}">
       <text>
         <r>
           <rPr>
@@ -2506,7 +2732,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M37" authorId="0" shapeId="0" xr:uid="{DCED5DFF-044A-4921-9C65-40BCB07BE401}">
+    <comment ref="M38" authorId="0" shapeId="0" xr:uid="{DCED5DFF-044A-4921-9C65-40BCB07BE401}">
       <text>
         <r>
           <rPr>
@@ -2586,7 +2812,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N37" authorId="0" shapeId="0" xr:uid="{54388763-F3A2-4348-BD10-BB9567BE1BD6}">
+    <comment ref="N38" authorId="0" shapeId="0" xr:uid="{54388763-F3A2-4348-BD10-BB9567BE1BD6}">
       <text>
         <r>
           <rPr>
@@ -2666,7 +2892,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O37" authorId="0" shapeId="0" xr:uid="{BB69DC05-6D8F-4916-A5BE-28127FA5ED45}">
+    <comment ref="O38" authorId="0" shapeId="0" xr:uid="{BB69DC05-6D8F-4916-A5BE-28127FA5ED45}">
       <text>
         <r>
           <rPr>
@@ -2746,7 +2972,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P37" authorId="0" shapeId="0" xr:uid="{083C9E3F-A057-4B33-AB86-07AA1E985C0D}">
+    <comment ref="P38" authorId="0" shapeId="0" xr:uid="{083C9E3F-A057-4B33-AB86-07AA1E985C0D}">
       <text>
         <r>
           <rPr>
@@ -2804,7 +3030,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q37" authorId="0" shapeId="0" xr:uid="{5CFB3E72-67F1-45CA-AA33-83D7E0FEB327}">
+    <comment ref="Q38" authorId="0" shapeId="0" xr:uid="{5CFB3E72-67F1-45CA-AA33-83D7E0FEB327}">
       <text>
         <r>
           <rPr>
@@ -2862,7 +3088,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R37" authorId="0" shapeId="0" xr:uid="{BD6E6772-95A3-46A2-BD6F-DF0D6C3B1C93}">
+    <comment ref="R38" authorId="0" shapeId="0" xr:uid="{BD6E6772-95A3-46A2-BD6F-DF0D6C3B1C93}">
       <text>
         <r>
           <rPr>
@@ -2920,7 +3146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S37" authorId="0" shapeId="0" xr:uid="{0F60EE06-13E2-4E08-A4F1-5C272396AC26}">
+    <comment ref="S38" authorId="0" shapeId="0" xr:uid="{0F60EE06-13E2-4E08-A4F1-5C272396AC26}">
       <text>
         <r>
           <rPr>
@@ -2936,7 +3162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A59" authorId="0" shapeId="0" xr:uid="{6F6EA05E-79A5-4221-8F31-4196F826573E}">
+    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{6F6EA05E-79A5-4221-8F31-4196F826573E}">
       <text>
         <r>
           <rPr>
@@ -2950,7 +3176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{4656F1B0-A803-4CE7-B6AD-DD7E0AECE077}">
+    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{4656F1B0-A803-4CE7-B6AD-DD7E0AECE077}">
       <text>
         <r>
           <rPr>
@@ -2964,7 +3190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{BFA6D1D6-A9C6-487C-93B1-D308A85B2F4C}">
+    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{BFA6D1D6-A9C6-487C-93B1-D308A85B2F4C}">
       <text>
         <r>
           <rPr>
@@ -2988,7 +3214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{7DF7F951-E3AA-46C9-9400-4FA052D43573}">
+    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{7DF7F951-E3AA-46C9-9400-4FA052D43573}">
       <text>
         <r>
           <rPr>
@@ -3002,7 +3228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{2594ED88-E6B7-439D-A482-5C038E3BCB4A}">
+    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{2594ED88-E6B7-439D-A482-5C038E3BCB4A}">
       <text>
         <r>
           <rPr>
@@ -3335,7 +3561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A65" authorId="0" shapeId="0" xr:uid="{494BCB97-31DA-4563-A050-36DD8A467D3F}">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{494BCB97-31DA-4563-A050-36DD8A467D3F}">
       <text>
         <r>
           <rPr>
@@ -3427,7 +3653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{6BCE8D0B-7F45-475A-86B8-E2D963D86E30}">
+    <comment ref="A67" authorId="0" shapeId="0" xr:uid="{6BCE8D0B-7F45-475A-86B8-E2D963D86E30}">
       <text>
         <r>
           <rPr>
@@ -3444,98 +3670,6 @@
 Read alignment software, version, parameters;
 Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
 etc.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A67" authorId="0" shapeId="0" xr:uid="{28C77FE7-DBD7-4513-B8B9-86AC1FA288D3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Provide details of how processed data files were generated. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Steps may include:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Base-calling software, version, parameters;
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Data filtering steps;
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Read alignment software, version, parameters;
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Additional processing software (e.g., peak-calling, abundance measurement), version, parameters;
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">etc.
 </t>
         </r>
       </text>
@@ -8711,7 +8845,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="784">
   <si>
     <t>SAMPLES</t>
   </si>
@@ -11290,9 +11424,6 @@
     <t>Joel, S, Griffitts</t>
   </si>
   <si>
-    <t>Bradford, K, Berges</t>
-  </si>
-  <si>
     <t>Sample 9</t>
   </si>
   <si>
@@ -11345,9 +11476,6 @@
   </si>
   <si>
     <t>Infected</t>
-  </si>
-  <si>
-    <t>Illumina's NovaSeq 6000</t>
   </si>
   <si>
     <t>I_4hrsS1_Data2.fq.gz</t>
@@ -11434,107 +11562,16 @@
 solution (100 U/mL Penicillin and 100ug/mL Streptomycin), at 41C in a humidified atmosphere with 5% CO2. When infected or mock infected, cells were maintained in 1:1 serum-reduced Leibovitz's L15/McCoy's 5A media (SRLM) with 2.5% FBS, 5% ChS, 1.2% TPB, and 1% antibiotics solution (100 U/mL Penicillin and 100ug/mL Streptomycin)</t>
   </si>
   <si>
-    <t>A commercially available THEV live vaccine was purchased from Hygieia Biological Labs. The stock virus was titrated using an 
-in-house qPCR assay with titer expressed as genome copy number(GCN)/mL, similar to Mahshoub et al
-(https://doi.org/10.1016/j.jviromet.2016.11.002) with modifications. Cells were infected in triplicates at a multiplicity of infection (MOI) 
-of 100 GCN/cell, incubate at 41C for 1 hour, and washed three times to get rid of free virion particles. Samples in triplicates were 
-harvested at 4-, 12-, 24-, and 72-h.p.i for total RNA extraction and RNA-sequencing</t>
-  </si>
-  <si>
     <t>Poly(A) RNA sequencing library was prepared following Illumina’s TruSeq-stranded-mRNA sample preparation protocol. 1ug of total
 RNA was used for this library construction</t>
   </si>
   <si>
-    <t>Hemorrhagic enteritis (HE) is a disease affecting 6-12-week-old turkeys characterized by immunosuppression (IS) and bloody diarrhea. This disease is caused by Turkey Hemorrhagic Enteritis Virus (THEV) of which avirulent strains (THEV-A) that do not cause HE but retain the immunosuppressive ability have been isolated. The THEV-A Virginia Avirulent Strain (VAS) is still used as a live vaccine despite its immunosuppressive properties. We have performed the first RNA-sequencing experiment characterizing THEV’s transcriptome, yielding the most detailed insight into THEV gene expression, to set the stage for further experimentation with specific viral genes that may mediate IS. After infecting a turkey B-cell line (MDTC-RP19) with the VAS vaccine strain, samples in triplicates were collected at 4-, 12-, 24-, and 72-hours post-infection. Total RNA was subsequently extracted, and poly-A-tailed mRNA sequencing done. After trimming the raw sequencing reads with the Trim-galore, reads were mapped to the THEV genome using Hisat2 and transcripts assembled with StringTie. We identified 29 transcripts from our RNA-seq data all of which consisted of novel exons albeit some exons matched the predicted ORFs. The three predicted splice junctions were also corroborated in our data. We performed PCR amplification of THEV cDNA, cloned the PCR products, and Sanger sequencing was used to validate all identified splice junctions. During validation, we identified 4 additional transcripts some of which were further validated by 3'RACE data. Thus, the transcriptome of THEV consists of 33 unique transcripts with the coding capacity for all predicted ORFs. However, we found 8 predicted ORFs to be incomplete as either an upstream, in-frame start codon was identified or additional coding exons were found, making the actual expressed versions of these ORFs longer. We also identified 7 novel unpredicted ORFs that could be encoded by some transcripts; albeit it is beyond the scope of this manuscript to investigate whether they are indeed expressed. In keeping with all Adenoviruses, our data shows that all THEV transcripts are spliced, and organized in transcription units under the control of their cognate promoter.</t>
-  </si>
-  <si>
     <t>A THEV vaccine was used to infect a turkey cell line (MDTC-RP19) and harvested at 4-, 12-, 24-, and 72-hpi in triplicates. RNA-seq was done for polyA-tailed mRNA</t>
   </si>
   <si>
-    <t>thev_subset_4hrsS1.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_4hrsS2.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_4hrsS3.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_12hrsS1.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_12hrsS3.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_24hrsS1.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_24hrsS2.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_24hrsS3.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_72hrsS1.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_72hrsS2.bam</t>
-  </si>
-  <si>
-    <t>thev_subset_72hrsS3.bam</t>
-  </si>
-  <si>
-    <t>thev_trxpt_fpkm.txt</t>
-  </si>
-  <si>
-    <t>thev_unq_juncs_geo.txt</t>
-  </si>
-  <si>
     <t>Reads were trimmed with the Trim-galore (v0.6.6) program to achieve an overall Mean Sequence Quality of 36</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Trimmed reads were mapped simultaneously to the complete genomic sequence of avirulent turkey hemorrhagic enteritis virus (THEV) and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Meleagris gallopavo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> using Hisat2  (v 2.2.1), and reads mapping to THEV filtered as new BAM files with Samtools (v1.16.1)</t>
-    </r>
-  </si>
-  <si>
-    <t>StringTie (v 2.2.1) was used to assemble the transcriptome using a GTF file derived from a gff3 file obtained from NCBI, 
-which contains the predicted ORFs of THEV as a guide. GFFCOMPARE (v0.12.6) was used to merge all transcripts from all time points without redundancy.</t>
-  </si>
-  <si>
-    <t>StringTie set to expression estimation mode was used to calculate FPKM scores for all transcripts after which Ballgown (ve2.33.0)
- in R was used to perform the statistical analysis on the transcript expression levels.</t>
-  </si>
-  <si>
-    <t>Regtools (1.0.0) was used to count all junctions, the reads supporting them, and extract all other information related to the junction.</t>
-  </si>
-  <si>
-    <t>BAM files of reads mapped to the THEV genome for each replicates of each time point</t>
-  </si>
-  <si>
-    <t>tab-delimted text file containing the FPKM values for each sample</t>
-  </si>
-  <si>
-    <t>tab-delimted text file containing combined unique junctions from all replicates and time points</t>
-  </si>
-  <si>
     <t>370ffb67764764f6ec524c52e8ac6d1c</t>
   </si>
   <si>
@@ -11601,49 +11638,7 @@
     <t>7ccead3d1050328726325938bb48a979</t>
   </si>
   <si>
-    <t>2e237d5a83b0c1ae0058887c00b4344c</t>
-  </si>
-  <si>
-    <t>f0f7b7f46019ec1377ddb5ec2589b7d3</t>
-  </si>
-  <si>
-    <t>35947e8379925c08fe2751fbed79af76</t>
-  </si>
-  <si>
-    <t>d17a40c46df3d526314bcb33d317f6b9</t>
-  </si>
-  <si>
-    <t>8f7104dbf6ea9aee9c87ce591b9064a8</t>
-  </si>
-  <si>
-    <t>59014d0e82d3f488fe709771c81ba1eb</t>
-  </si>
-  <si>
-    <t>58febf81c3238f2d1dacd47d30a1a772</t>
-  </si>
-  <si>
-    <t>c912dffb567a6ced5eba2296dbc6ac21</t>
-  </si>
-  <si>
-    <t>5f4a50e884fb4eb7f01cf3002f7f7868</t>
-  </si>
-  <si>
-    <t>427d345d1d7529f98fb216daa1367c78</t>
-  </si>
-  <si>
-    <t>9f3ff87872d92173697412b531758743</t>
-  </si>
-  <si>
-    <t>e4ecc8e6093071441f2249cebde9a45b</t>
-  </si>
-  <si>
-    <t>c6c7426b7b2b9ea84dee33daec801229</t>
-  </si>
-  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Host Turkey B-cell Transcriptomics During THEV Infection Highlights Upregulated Cell Death and Breakdown Pathways That May Mediate Immunosuppression</t>
   </si>
   <si>
     <t>To understand the genetic basis by which THEV causes immunosuppression (IS) in infected turkeys, we performed an RNA-seq
@@ -11799,6 +11794,348 @@
   </si>
   <si>
     <t>melGal5</t>
+  </si>
+  <si>
+    <t>Turkey B-cell Transcriptome Profile During Turkey Hemorrhagic Enteritis Virus (THEV) Infection Highlights Upregulated Apoptosis and Breakdown Pathways That May Mediate Immunosuppression</t>
+  </si>
+  <si>
+    <t>A commercially available THEV live vaccine was purchased from Hygieia Biological Labs. The stock virus was titrated using an 
+in-house qPCR assay with titer expressed as genome copy number(GCN)/mL, similar to Mahshoub et al
+(https://doi.org/10.1016/j.jviromet.2016.11.002) with modifications. Cells were infected in triplicates at a multiplicity of infection (MOI) 
+of 100 GCN/cell, incubate at 41 centigrade for 1 hour, and washed three times to get rid of free virion particles. Samples in triplicates were 
+harvested at 4-, 12-, 24-, and 72-h.p.i for total RNA extraction and RNA-sequencing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Trimmed reads were mapped to </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Meleagris gallopavo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> using Hisat2  (v 2.2.1) and output SAM files were converted to BAM files using samtools (v 1.21).</t>
+    </r>
+  </si>
+  <si>
+    <t>StringTie (v 2.2.1), set to expression estimation mode was used to generate normalized gene expression estimates from the BAM files for genes in the reference GTF file after which the prepDE.py3 script was used to extract read count information from the StringTie gene expression files, providing an expression-count matrix for downstream DEG analysis.</t>
+  </si>
+  <si>
+    <t>Differential gene expression analysis between mock- and THEV-infected samples was performed using DESeq2 (v1.42.0) R package</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BAM files of reads mapped to the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>M. gallopavo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> genome for all replicates of each time point</t>
+    </r>
+  </si>
+  <si>
+    <t>comma-separated text file (csv) containing the FPKM values of all annotated M.gallopavo genes for each sample (gene count matrix)</t>
+  </si>
+  <si>
+    <t>comma-separated text files (csv) containing DESeq2 differential gene expression results (geneIDs/geneNames, sample names, log2fold changes, and adjusted p-values) for all timepoints 4, 12, 24, and 72 hours</t>
+  </si>
+  <si>
+    <t>sorted_I_4hrsS1.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_4hrsS2.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_4hrsS3.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_4hrsN1.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_4hrsN2.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_12hrsS1.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_12hrsS3.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_12hrsN1.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_12hrsN2.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_24hrsS1.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_24hrsS2.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_24hrsS3.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_24hrsN1.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_24hrsN2.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_72hrsS1.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_72hrsS2.bam</t>
+  </si>
+  <si>
+    <t>sorted_I_72hrsS3.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_72hrsN1.bam</t>
+  </si>
+  <si>
+    <t>sorted_U_72hrsN2.bam</t>
+  </si>
+  <si>
+    <t>genes_count_matrix.csv</t>
+  </si>
+  <si>
+    <t>total_4hrsDEGs.csv</t>
+  </si>
+  <si>
+    <t>total_12hrsDEGs.csv</t>
+  </si>
+  <si>
+    <t>total_24hrsDEGs.csv</t>
+  </si>
+  <si>
+    <t>total_72hrsDEGs.csv</t>
+  </si>
+  <si>
+    <t>b3f9ff6c86503088ecd7507ead8e1789</t>
+  </si>
+  <si>
+    <t>cfbbf2a2222ac1d3aefe060459953d76</t>
+  </si>
+  <si>
+    <t>47eb630ad4477e1c72c8b794f4998525</t>
+  </si>
+  <si>
+    <t>b9c3f078b2e8d1f353d911edc0e57be7</t>
+  </si>
+  <si>
+    <t>4ed731c5c100aedc262341c85e79ecbe</t>
+  </si>
+  <si>
+    <t>09917ec6729f7e48f76e5137fb8045f7</t>
+  </si>
+  <si>
+    <t>58784c63352756386004bb769bf74178</t>
+  </si>
+  <si>
+    <t>dab6ff88f7941a2e4c7f1893067d08b2</t>
+  </si>
+  <si>
+    <t>c09e9653d6541892c697c9a9f6857f1a</t>
+  </si>
+  <si>
+    <t>b05b12bf704f775671b8338ce7b8740a</t>
+  </si>
+  <si>
+    <t>8d455b4067c7eb7c1c800209f67f7c24</t>
+  </si>
+  <si>
+    <t>65c20abc678496fee2f17f99fc61cc06</t>
+  </si>
+  <si>
+    <t>eba2e8d6114f2ea71c2b312d88e6c19d</t>
+  </si>
+  <si>
+    <t>46b71ae43cbe7fa91369db8025ed7364</t>
+  </si>
+  <si>
+    <t>10921ddbcfd2adba3ef327ec31d3c853</t>
+  </si>
+  <si>
+    <t>1e9412c6d7dea66db4672d22ecd359be</t>
+  </si>
+  <si>
+    <t>0fbdc84d06bc2f10eccee39a6273ef59</t>
+  </si>
+  <si>
+    <t>e39d215ee9eba46b99bc7d463cfb53bf</t>
+  </si>
+  <si>
+    <t>baab8c6d25d2fe933422200dc8e4d306</t>
+  </si>
+  <si>
+    <t>0c88699163e4329995aca9b593cd211a</t>
+  </si>
+  <si>
+    <t>ae6b0bcbf66e8d07b649fc762a3c5381</t>
+  </si>
+  <si>
+    <t>728ee4e5f1f2d4fb1192b94e7d1a8d86</t>
+  </si>
+  <si>
+    <t>6f622aa6d991230e2c0a56cb253bd6d9</t>
+  </si>
+  <si>
+    <t>9bf94bc75515a79ed2f30575f5df67f4</t>
+  </si>
+  <si>
+    <t>ac92fa7898d9ae4b6801c28c7b277d86</t>
+  </si>
+  <si>
+    <t>9a4532ccfebc4f6699c3d070f29a28bd</t>
+  </si>
+  <si>
+    <t>a2b19378debf0d5f726d43479f0ecd9b</t>
+  </si>
+  <si>
+    <t>f9dd83d70750093afdd849fc7046dac2</t>
+  </si>
+  <si>
+    <t>1f0b10a561c9855caebfff01a16f85fd</t>
+  </si>
+  <si>
+    <t>0f1af3643d23b7e0f86bc2e14d9659bd</t>
+  </si>
+  <si>
+    <t>618a56f8ec62d8be55055180c18b37ec</t>
+  </si>
+  <si>
+    <t>9d2e5a54ba65d67ced04dc9a726524d4</t>
+  </si>
+  <si>
+    <t>4ae1fd45ea4d6630ab7afd4ce504bc41</t>
+  </si>
+  <si>
+    <t>14deb4c18fac77d18dbd8fe8679020c0</t>
+  </si>
+  <si>
+    <t>3b39ffd4e928846290a212ef7eb87e6d</t>
+  </si>
+  <si>
+    <t>2d1fc7cdc5728a12940904f8ee8fd22a</t>
+  </si>
+  <si>
+    <t>1ab78dc9c1aea5afba00e2ab4c9e9815</t>
+  </si>
+  <si>
+    <t>e061c41bc0a73de758d7f0ca21a54b98</t>
+  </si>
+  <si>
+    <t>3199c710b79359d4e851e90181e2e1e9</t>
+  </si>
+  <si>
+    <t>e8d428b9ac709a29accc071cf27b4a0a</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Background</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: Infection with Turkey Hemorrhagic Enteritis Virus (THEV) can cause hemorrhagic enteritis, which affects turkey poults. This disease is characterized by immunosuppression (IMS) and bloody droppings. The clinical disease usually lasts only a few days but secondary opportunistic infections due to THEV-induced IMS extend the duration of illness and mortality, which exacerbates economic losses. Although an avirulent THEV strain with only subclinical disease is used as a vaccine, some immunosuppressive properties remain in this prophylactic strain. To elucidate the mechanisms mediating THEV-induced IMS, we performed the first transcriptomic analysis of a THEV infection using bulk RNA-sequencing.     
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Methods:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> After infecting a turkey B-cell line with the vaccine strain, samples in triplicates were collected at 4-, 12-, 24-, and 72-hours post-infection (hpi). Total RNA was extracted, and poly-Adenylated-tailed mRNAs were sequenced. Reads were mapped to the host turkey genome after trimming and gene expression was quantified with StringTie. Differential gene expression was performed with DESeq2 followed by functional enrichment analysis with gprofiler2 and DAVID from NCBI. RT-qPCR of select genes was performed to validate the RNA-sequencing data.   
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Results:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> A total of 2,343 and 3,295 differentially expressed genes (DEGs) were identified at 12 hpi and 24 hpi, respectively. At 12 hpi, 1,079 genes were upregulated and 1,264 genes downregulated, whereas 1,512 genes were upregulated and 1,783 genes downregulated at 24 hpi. The DEGs contributed to multiple biological processes including apoptosis, ER unfolded protein response, and cell maintenance. Multiple pro-apoptotic genes, including APAF1, BNIP3L, BMF, BAK1, RIPK1, and FAS were upregulated. Genes that play a role in ER stress-induced unfolded protein response including VCP, UFD1, EDEM1, EDEM3, and ATF4 were also upregulated and may contribute to apoptosis.    
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Conclusions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Our data suggest that several biological processes and pathways including apoptosis, immune response, ER response to stress, ubiquitin-dependent protein catabolic process, and repression of essential cellular maintenance are important aspects of the host cell response to THEV infection. It is possible that interplay between multiple processes may mediate apoptosis of infected B-cells, leading to IMS.</t>
+    </r>
+  </si>
+  <si>
+    <t>Bradford, K, Berges</t>
   </si>
 </sst>
 </file>
@@ -12406,7 +12743,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -12621,18 +12958,10 @@
     <xf numFmtId="11" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
+    <xf numFmtId="11" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -12647,6 +12976,22 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="28">
@@ -12679,17 +13024,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Normal 3" xfId="27" xr:uid="{F4D64B01-3AA2-4CE5-A7EE-64332280C940}"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -12859,13 +13194,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>371292</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>120687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>526256</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>31487</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -12932,13 +13267,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>164306</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>607219</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>142877</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -13186,13 +13521,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>392906</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>392906</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>161282</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -17034,14 +17369,14 @@
   </sheetPr>
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="107" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="83.6640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.6640625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="135.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="192.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="8" customWidth="1"/>
     <col min="5" max="8" width="17.6640625" style="8" customWidth="1"/>
@@ -17050,7 +17385,8 @@
     <col min="11" max="11" width="25.5" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="23.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="23.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="20" width="20" style="8" customWidth="1"/>
     <col min="21" max="16384" width="83.6640625" style="8"/>
   </cols>
@@ -17164,17 +17500,17 @@
       <c r="A11" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="B11" s="51" t="s">
-        <v>709</v>
+      <c r="B11" s="74" t="s">
+        <v>710</v>
       </c>
       <c r="C11" s="51"/>
     </row>
-    <row r="12" spans="1:18" ht="262" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="177" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>349</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>650</v>
+        <v>782</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="42" x14ac:dyDescent="0.2">
@@ -17182,23 +17518,23 @@
         <v>350</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="28" x14ac:dyDescent="0.2">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>350</v>
       </c>
       <c r="B14" s="42" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="42" x14ac:dyDescent="0.2">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>350</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>711</v>
+        <v>673</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="28" x14ac:dyDescent="0.2">
@@ -17206,15 +17542,15 @@
         <v>350</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="28" x14ac:dyDescent="0.2">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>350</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>713</v>
+        <v>675</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
@@ -17222,7 +17558,7 @@
         <v>236</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
@@ -17253,14 +17589,17 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>783</v>
+      </c>
+      <c r="E22" s="27"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
@@ -17281,72 +17620,53 @@
       <c r="A29" s="29"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="30"/>
-      <c r="P30" s="30"/>
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
-    </row>
-    <row r="31" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+      <c r="A30" s="29"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="30"/>
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30"/>
+      <c r="R31" s="30"/>
+    </row>
+    <row r="32" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="24"/>
-      <c r="O31" s="24"/>
-      <c r="P31" s="24"/>
-      <c r="Q31" s="24"/>
-      <c r="R31" s="25"/>
-    </row>
-    <row r="32" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
-      <c r="O32" s="10"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
-      <c r="R32" s="11"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="25"/>
     </row>
     <row r="33" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>251</v>
+        <v>28</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -17366,31 +17686,31 @@
       <c r="Q33" s="10"/>
       <c r="R33" s="11"/>
     </row>
-    <row r="34" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="52" t="s">
-        <v>252</v>
-      </c>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="52"/>
-      <c r="O34" s="52"/>
-      <c r="P34" s="52"/>
-      <c r="Q34" s="52"/>
-      <c r="R34" s="53"/>
+    <row r="34" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="11"/>
     </row>
     <row r="35" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="52" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
@@ -17410,160 +17730,133 @@
       <c r="Q35" s="52"/>
       <c r="R35" s="53"/>
     </row>
-    <row r="36" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="58" t="s">
+    <row r="36" spans="1:19" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="52" t="s">
+        <v>253</v>
+      </c>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="53"/>
+    </row>
+    <row r="37" spans="1:19" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="58" t="s">
         <v>581</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="58"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="59"/>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A37" s="44" t="s">
+      <c r="B37" s="58"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="59"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A38" s="44" t="s">
         <v>351</v>
       </c>
-      <c r="B37" s="44" t="s">
+      <c r="B38" s="44" t="s">
         <v>348</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C38" s="45" t="s">
         <v>352</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D38" s="31" t="s">
         <v>353</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E38" s="31" t="s">
         <v>355</v>
       </c>
-      <c r="F37" s="31" t="s">
+      <c r="F38" s="31" t="s">
         <v>356</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G38" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="31" t="s">
+      <c r="H38" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="44" t="s">
+      <c r="I38" s="44" t="s">
         <v>357</v>
       </c>
-      <c r="J37" s="44" t="s">
+      <c r="J38" s="44" t="s">
         <v>358</v>
       </c>
-      <c r="K37" s="44" t="s">
+      <c r="K38" s="44" t="s">
         <v>359</v>
       </c>
-      <c r="L37" s="44" t="s">
+      <c r="L38" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="M37" s="31" t="s">
+      <c r="M38" s="31" t="s">
         <v>369</v>
       </c>
-      <c r="N37" s="31" t="s">
+      <c r="N38" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="O37" s="31" t="s">
+      <c r="O38" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="P37" s="31" t="s">
+      <c r="P38" s="31" t="s">
         <v>370</v>
       </c>
-      <c r="Q37" s="31" t="s">
+      <c r="Q38" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="R37" s="31" t="s">
+      <c r="R38" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="S37" s="31" t="s">
+      <c r="S38" s="31" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A38" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>605</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>615</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>616</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>617</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>618</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>619</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J38" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="14" t="s">
-        <v>620</v>
-      </c>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14" t="s">
-        <v>652</v>
-      </c>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14" t="s">
-        <v>664</v>
-      </c>
-      <c r="P38" s="14" t="s">
-        <v>622</v>
-      </c>
-      <c r="Q38" s="14" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C39" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E39" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E39" s="14" t="s">
+      <c r="F39" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="G39" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="H39" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H39" s="14" t="s">
-        <v>619</v>
       </c>
       <c r="I39" s="14" t="s">
         <v>9</v>
@@ -17571,48 +17864,50 @@
       <c r="J39" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K39" s="14" t="s">
-        <v>620</v>
+      <c r="K39" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L39" s="14"/>
       <c r="M39" s="14" t="s">
-        <v>653</v>
-      </c>
-      <c r="N39" s="14"/>
+        <v>718</v>
+      </c>
+      <c r="N39" s="14" t="s">
+        <v>737</v>
+      </c>
       <c r="O39" s="14" t="s">
-        <v>664</v>
+        <v>738</v>
       </c>
       <c r="P39" s="14" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="Q39" s="14" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>643</v>
+        <v>605</v>
       </c>
       <c r="C40" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E40" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E40" s="14" t="s">
+      <c r="F40" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="G40" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="H40" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H40" s="14" t="s">
-        <v>619</v>
       </c>
       <c r="I40" s="14" t="s">
         <v>9</v>
@@ -17620,48 +17915,50 @@
       <c r="J40" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K40" s="14" t="s">
-        <v>620</v>
+      <c r="K40" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L40" s="14"/>
       <c r="M40" s="14" t="s">
-        <v>654</v>
-      </c>
-      <c r="N40" s="14"/>
+        <v>719</v>
+      </c>
+      <c r="N40" s="14" t="s">
+        <v>737</v>
+      </c>
       <c r="O40" s="14" t="s">
-        <v>664</v>
-      </c>
-      <c r="P40" s="8" t="s">
-        <v>625</v>
+        <v>738</v>
+      </c>
+      <c r="P40" s="14" t="s">
+        <v>621</v>
       </c>
       <c r="Q40" s="14" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>714</v>
+        <v>641</v>
       </c>
       <c r="C41" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E41" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D41" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E41" s="14" t="s">
+      <c r="F41" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="G41" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="H41" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>730</v>
       </c>
       <c r="I41" s="14" t="s">
         <v>9</v>
@@ -17669,48 +17966,50 @@
       <c r="J41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K41" s="14" t="s">
-        <v>620</v>
+      <c r="K41" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L41" s="14"/>
       <c r="M41" s="14" t="s">
-        <v>652</v>
-      </c>
-      <c r="N41" s="14"/>
+        <v>720</v>
+      </c>
+      <c r="N41" s="14" t="s">
+        <v>737</v>
+      </c>
       <c r="O41" s="14" t="s">
-        <v>664</v>
-      </c>
-      <c r="P41" s="14" t="s">
-        <v>731</v>
+        <v>738</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>623</v>
       </c>
       <c r="Q41" s="14" t="s">
-        <v>739</v>
+        <v>624</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>716</v>
+        <v>676</v>
       </c>
       <c r="C42" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E42" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E42" s="14" t="s">
+      <c r="F42" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="G42" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G42" s="14" t="s">
-        <v>618</v>
-      </c>
       <c r="H42" s="14" t="s">
-        <v>730</v>
+        <v>692</v>
       </c>
       <c r="I42" s="14" t="s">
         <v>9</v>
@@ -17718,48 +18017,50 @@
       <c r="J42" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K42" s="14" t="s">
-        <v>620</v>
+      <c r="K42" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L42" s="14"/>
       <c r="M42" s="14" t="s">
-        <v>652</v>
-      </c>
-      <c r="N42" s="14"/>
+        <v>721</v>
+      </c>
+      <c r="N42" s="14" t="s">
+        <v>737</v>
+      </c>
       <c r="O42" s="14" t="s">
-        <v>664</v>
+        <v>738</v>
       </c>
       <c r="P42" s="14" t="s">
-        <v>732</v>
+        <v>693</v>
       </c>
       <c r="Q42" s="14" t="s">
-        <v>740</v>
+        <v>701</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>607</v>
+        <v>678</v>
       </c>
       <c r="C43" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E43" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D43" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E43" s="14" t="s">
+      <c r="F43" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="G43" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G43" s="14" t="s">
-        <v>618</v>
-      </c>
       <c r="H43" s="14" t="s">
-        <v>619</v>
+        <v>692</v>
       </c>
       <c r="I43" s="14" t="s">
         <v>9</v>
@@ -17767,50 +18068,50 @@
       <c r="J43" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K43" s="14" t="s">
-        <v>620</v>
+      <c r="K43" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L43" s="14"/>
       <c r="M43" s="14" t="s">
-        <v>655</v>
+        <v>722</v>
       </c>
       <c r="N43" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O43" s="14" t="s">
-        <v>664</v>
+        <v>738</v>
       </c>
       <c r="P43" s="14" t="s">
-        <v>627</v>
+        <v>694</v>
       </c>
       <c r="Q43" s="14" t="s">
-        <v>628</v>
+        <v>702</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="37" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C44" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D44" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E44" s="14" t="s">
+      <c r="F44" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="G44" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="H44" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H44" s="14" t="s">
-        <v>619</v>
       </c>
       <c r="I44" s="14" t="s">
         <v>9</v>
@@ -17818,50 +18119,50 @@
       <c r="J44" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K44" s="14" t="s">
-        <v>620</v>
+      <c r="K44" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L44" s="14"/>
       <c r="M44" s="14" t="s">
-        <v>656</v>
+        <v>723</v>
       </c>
       <c r="N44" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O44" s="14" t="s">
-        <v>664</v>
+        <v>739</v>
       </c>
       <c r="P44" s="14" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="Q44" s="14" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>715</v>
+        <v>607</v>
       </c>
       <c r="C45" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E45" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D45" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E45" s="14" t="s">
+      <c r="F45" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="G45" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="H45" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>730</v>
       </c>
       <c r="I45" s="14" t="s">
         <v>9</v>
@@ -17869,50 +18170,50 @@
       <c r="J45" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K45" s="14" t="s">
-        <v>620</v>
+      <c r="K45" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L45" s="14"/>
       <c r="M45" s="14" t="s">
-        <v>655</v>
+        <v>724</v>
       </c>
       <c r="N45" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O45" s="14" t="s">
-        <v>664</v>
+        <v>739</v>
       </c>
       <c r="P45" s="14" t="s">
-        <v>733</v>
+        <v>627</v>
       </c>
       <c r="Q45" s="14" t="s">
-        <v>741</v>
+        <v>628</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="37" t="s">
-        <v>602</v>
+        <v>73</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>717</v>
+        <v>677</v>
       </c>
       <c r="C46" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E46" s="14" t="s">
+      <c r="F46" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="G46" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G46" s="14" t="s">
-        <v>618</v>
-      </c>
       <c r="H46" s="14" t="s">
-        <v>730</v>
+        <v>692</v>
       </c>
       <c r="I46" s="14" t="s">
         <v>9</v>
@@ -17920,50 +18221,50 @@
       <c r="J46" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K46" s="14" t="s">
-        <v>620</v>
+      <c r="K46" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L46" s="14"/>
       <c r="M46" s="14" t="s">
-        <v>655</v>
+        <v>725</v>
       </c>
       <c r="N46" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O46" s="14" t="s">
-        <v>664</v>
+        <v>739</v>
       </c>
       <c r="P46" s="14" t="s">
-        <v>734</v>
+        <v>695</v>
       </c>
       <c r="Q46" s="14" t="s">
-        <v>742</v>
+        <v>703</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="37" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>609</v>
+        <v>679</v>
       </c>
       <c r="C47" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E47" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E47" s="14" t="s">
+      <c r="F47" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="G47" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G47" s="14" t="s">
-        <v>618</v>
-      </c>
       <c r="H47" s="14" t="s">
-        <v>619</v>
+        <v>692</v>
       </c>
       <c r="I47" s="14" t="s">
         <v>9</v>
@@ -17971,51 +18272,50 @@
       <c r="J47" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K47" s="14" t="s">
-        <v>620</v>
+      <c r="K47" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L47" s="14"/>
       <c r="M47" s="14" t="s">
-        <v>657</v>
+        <v>726</v>
       </c>
       <c r="N47" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O47" s="14" t="s">
-        <v>664</v>
+        <v>739</v>
       </c>
       <c r="P47" s="14" t="s">
-        <v>632</v>
+        <v>696</v>
       </c>
       <c r="Q47" s="14" t="s">
-        <v>631</v>
-      </c>
-      <c r="R47" s="14"/>
+        <v>704</v>
+      </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="37" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C48" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E48" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E48" s="14" t="s">
+      <c r="F48" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="G48" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="H48" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>619</v>
       </c>
       <c r="I48" s="14" t="s">
         <v>9</v>
@@ -18023,51 +18323,51 @@
       <c r="J48" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K48" s="14" t="s">
-        <v>620</v>
+      <c r="K48" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L48" s="14"/>
       <c r="M48" s="14" t="s">
-        <v>658</v>
+        <v>727</v>
       </c>
       <c r="N48" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O48" s="14" t="s">
-        <v>664</v>
+        <v>740</v>
       </c>
       <c r="P48" s="14" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="Q48" s="14" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="R48" s="14"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="37" t="s">
-        <v>718</v>
+        <v>603</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C49" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E49" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E49" s="14" t="s">
+      <c r="F49" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="G49" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="H49" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>619</v>
       </c>
       <c r="I49" s="14" t="s">
         <v>9</v>
@@ -18075,51 +18375,51 @@
       <c r="J49" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K49" s="14" t="s">
-        <v>620</v>
+      <c r="K49" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L49" s="14"/>
       <c r="M49" s="14" t="s">
-        <v>659</v>
+        <v>728</v>
       </c>
       <c r="N49" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O49" s="14" t="s">
-        <v>664</v>
+        <v>740</v>
       </c>
       <c r="P49" s="14" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="Q49" s="14" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="R49" s="14"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="37" t="s">
-        <v>719</v>
+        <v>680</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>722</v>
+        <v>610</v>
       </c>
       <c r="C50" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D50" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E50" s="14" t="s">
+      <c r="F50" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="G50" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="H50" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>730</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>9</v>
@@ -18127,51 +18427,51 @@
       <c r="J50" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K50" s="14" t="s">
-        <v>620</v>
+      <c r="K50" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L50" s="14"/>
       <c r="M50" s="14" t="s">
-        <v>659</v>
+        <v>729</v>
       </c>
       <c r="N50" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O50" s="14" t="s">
-        <v>664</v>
+        <v>740</v>
       </c>
       <c r="P50" s="14" t="s">
-        <v>735</v>
+        <v>633</v>
       </c>
       <c r="Q50" s="14" t="s">
-        <v>743</v>
+        <v>634</v>
       </c>
       <c r="R50" s="14"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" s="37" t="s">
-        <v>720</v>
+        <v>681</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>723</v>
+        <v>684</v>
       </c>
       <c r="C51" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E51" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D51" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E51" s="14" t="s">
+      <c r="F51" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="G51" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G51" s="14" t="s">
-        <v>618</v>
-      </c>
       <c r="H51" s="14" t="s">
-        <v>730</v>
+        <v>692</v>
       </c>
       <c r="I51" s="14" t="s">
         <v>9</v>
@@ -18179,51 +18479,51 @@
       <c r="J51" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K51" s="14" t="s">
-        <v>620</v>
+      <c r="K51" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L51" s="14"/>
       <c r="M51" s="14" t="s">
-        <v>659</v>
+        <v>730</v>
       </c>
       <c r="N51" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O51" s="14" t="s">
-        <v>664</v>
+        <v>740</v>
       </c>
       <c r="P51" s="14" t="s">
-        <v>736</v>
+        <v>697</v>
       </c>
       <c r="Q51" s="14" t="s">
-        <v>744</v>
+        <v>705</v>
       </c>
       <c r="R51" s="14"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" s="37" t="s">
-        <v>721</v>
+        <v>682</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>612</v>
+        <v>685</v>
       </c>
       <c r="C52" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E52" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D52" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E52" s="14" t="s">
+      <c r="F52" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="G52" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G52" s="14" t="s">
-        <v>618</v>
-      </c>
       <c r="H52" s="14" t="s">
-        <v>619</v>
+        <v>692</v>
       </c>
       <c r="I52" s="14" t="s">
         <v>9</v>
@@ -18231,51 +18531,51 @@
       <c r="J52" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K52" s="14" t="s">
-        <v>620</v>
+      <c r="K52" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L52" s="14"/>
       <c r="M52" s="14" t="s">
-        <v>660</v>
+        <v>731</v>
       </c>
       <c r="N52" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O52" s="14" t="s">
-        <v>664</v>
+        <v>740</v>
       </c>
       <c r="P52" s="14" t="s">
-        <v>637</v>
+        <v>698</v>
       </c>
       <c r="Q52" s="14" t="s">
-        <v>638</v>
+        <v>706</v>
       </c>
       <c r="R52" s="14"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="37" t="s">
-        <v>724</v>
+        <v>683</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C53" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D53" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E53" s="14" t="s">
+      <c r="F53" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="G53" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="H53" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>619</v>
       </c>
       <c r="I53" s="14" t="s">
         <v>9</v>
@@ -18283,51 +18583,51 @@
       <c r="J53" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K53" s="14" t="s">
-        <v>620</v>
+      <c r="K53" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L53" s="14"/>
       <c r="M53" s="14" t="s">
-        <v>661</v>
+        <v>732</v>
       </c>
       <c r="N53" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O53" s="14" t="s">
-        <v>664</v>
+        <v>741</v>
       </c>
       <c r="P53" s="14" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="Q53" s="14" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="R53" s="14"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" s="37" t="s">
-        <v>725</v>
+        <v>686</v>
       </c>
       <c r="B54" s="14" t="s">
+        <v>612</v>
+      </c>
+      <c r="C54" s="14" t="s">
         <v>614</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="D54" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E54" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D54" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E54" s="14" t="s">
+      <c r="F54" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="G54" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="H54" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>619</v>
       </c>
       <c r="I54" s="14" t="s">
         <v>9</v>
@@ -18335,51 +18635,51 @@
       <c r="J54" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K54" s="14" t="s">
-        <v>620</v>
+      <c r="K54" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L54" s="14"/>
       <c r="M54" s="14" t="s">
-        <v>662</v>
+        <v>733</v>
       </c>
       <c r="N54" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O54" s="14" t="s">
-        <v>664</v>
+        <v>741</v>
       </c>
       <c r="P54" s="14" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="Q54" s="14" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="R54" s="14"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A55" s="37" t="s">
-        <v>726</v>
+        <v>687</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>728</v>
+        <v>613</v>
       </c>
       <c r="C55" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E55" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D55" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E55" s="14" t="s">
+      <c r="F55" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="G55" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="H55" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="H55" s="14" t="s">
-        <v>730</v>
       </c>
       <c r="I55" s="14" t="s">
         <v>9</v>
@@ -18387,51 +18687,51 @@
       <c r="J55" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K55" s="14" t="s">
-        <v>620</v>
+      <c r="K55" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L55" s="14"/>
       <c r="M55" s="14" t="s">
-        <v>662</v>
+        <v>734</v>
       </c>
       <c r="N55" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O55" s="14" t="s">
-        <v>664</v>
+        <v>741</v>
       </c>
       <c r="P55" s="14" t="s">
-        <v>737</v>
+        <v>639</v>
       </c>
       <c r="Q55" s="14" t="s">
-        <v>745</v>
+        <v>640</v>
       </c>
       <c r="R55" s="14"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="37" t="s">
-        <v>727</v>
+        <v>688</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>729</v>
+        <v>690</v>
       </c>
       <c r="C56" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E56" s="14" t="s">
         <v>615</v>
       </c>
-      <c r="D56" s="14" t="s">
-        <v>708</v>
-      </c>
-      <c r="E56" s="14" t="s">
+      <c r="F56" s="14" t="s">
         <v>616</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="G56" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="G56" s="14" t="s">
-        <v>618</v>
-      </c>
       <c r="H56" s="14" t="s">
-        <v>730</v>
+        <v>692</v>
       </c>
       <c r="I56" s="14" t="s">
         <v>9</v>
@@ -18439,101 +18739,129 @@
       <c r="J56" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K56" s="14" t="s">
-        <v>620</v>
+      <c r="K56" s="85" t="s">
+        <v>265</v>
       </c>
       <c r="L56" s="14"/>
       <c r="M56" s="14" t="s">
-        <v>662</v>
+        <v>735</v>
       </c>
       <c r="N56" s="14" t="s">
-        <v>663</v>
+        <v>737</v>
       </c>
       <c r="O56" s="14" t="s">
-        <v>664</v>
+        <v>741</v>
       </c>
       <c r="P56" s="14" t="s">
-        <v>738</v>
+        <v>699</v>
       </c>
       <c r="Q56" s="14" t="s">
-        <v>746</v>
+        <v>707</v>
       </c>
       <c r="R56" s="14"/>
     </row>
-    <row r="57" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="9" t="s">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A57" s="37" t="s">
+        <v>689</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>691</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>617</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>692</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J57" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K57" s="85" t="s">
+        <v>265</v>
+      </c>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14" t="s">
+        <v>736</v>
+      </c>
+      <c r="N57" s="14" t="s">
+        <v>737</v>
+      </c>
+      <c r="O57" s="14" t="s">
+        <v>741</v>
+      </c>
+      <c r="P57" s="14" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q57" s="14" t="s">
+        <v>708</v>
+      </c>
+      <c r="R57" s="14"/>
+    </row>
+    <row r="58" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="24"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
-      <c r="K57" s="24"/>
-      <c r="L57" s="24"/>
-      <c r="M57" s="24"/>
-      <c r="N57" s="24"/>
-      <c r="O57" s="24"/>
-      <c r="P57" s="24"/>
-      <c r="Q57" s="24"/>
-      <c r="R57" s="25"/>
-    </row>
-    <row r="58" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
+      <c r="K58" s="24"/>
+      <c r="L58" s="24"/>
+      <c r="M58" s="24"/>
+      <c r="N58" s="24"/>
+      <c r="O58" s="24"/>
+      <c r="P58" s="24"/>
+      <c r="Q58" s="24"/>
+      <c r="R58" s="25"/>
+    </row>
+    <row r="59" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
         <v>588</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="10"/>
-      <c r="P58" s="10"/>
-      <c r="Q58" s="10"/>
-      <c r="R58" s="11"/>
-    </row>
-    <row r="59" spans="1:18" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="13" t="s">
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10"/>
+      <c r="O59" s="10"/>
+      <c r="P59" s="10"/>
+      <c r="Q59" s="10"/>
+      <c r="R59" s="11"/>
+    </row>
+    <row r="60" spans="1:18" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="13" t="s">
         <v>360</v>
       </c>
-      <c r="B59" s="43" t="s">
-        <v>647</v>
-      </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="N59" s="14"/>
-      <c r="O59" s="14"/>
-      <c r="P59" s="14"/>
-      <c r="Q59" s="14"/>
-      <c r="R59" s="14"/>
-    </row>
-    <row r="60" spans="1:18" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
-        <v>361</v>
-      </c>
       <c r="B60" s="43" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -18552,12 +18880,12 @@
       <c r="Q60" s="14"/>
       <c r="R60" s="14"/>
     </row>
-    <row r="61" spans="1:18" ht="28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>646</v>
+        <v>711</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
@@ -18576,12 +18904,12 @@
       <c r="Q61" s="14"/>
       <c r="R61" s="14"/>
     </row>
-    <row r="62" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A62" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="B62" s="72" t="s">
-        <v>649</v>
+        <v>362</v>
+      </c>
+      <c r="B62" s="43" t="s">
+        <v>644</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
@@ -18600,12 +18928,12 @@
       <c r="Q62" s="14"/>
       <c r="R62" s="14"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" ht="28" x14ac:dyDescent="0.15">
       <c r="A63" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>645</v>
+        <v>363</v>
+      </c>
+      <c r="B63" s="72" t="s">
+        <v>646</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
@@ -18625,8 +18953,12 @@
       <c r="R63" s="14"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="13"/>
-      <c r="B64" s="14"/>
+      <c r="A64" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>643</v>
+      </c>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
@@ -18645,12 +18977,8 @@
       <c r="R64" s="14"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A65" s="13" t="s">
-        <v>364</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>665</v>
-      </c>
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
@@ -18668,12 +18996,12 @@
       <c r="Q65" s="14"/>
       <c r="R65" s="14"/>
     </row>
-    <row r="66" spans="1:20" ht="42" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>565</v>
-      </c>
-      <c r="B66" s="43" t="s">
-        <v>666</v>
+        <v>364</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>648</v>
       </c>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
@@ -18692,12 +19020,12 @@
       <c r="Q66" s="14"/>
       <c r="R66" s="14"/>
     </row>
-    <row r="67" spans="1:20" ht="42" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" ht="14" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
         <v>565</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>667</v>
+        <v>712</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
@@ -18716,12 +19044,12 @@
       <c r="Q67" s="14"/>
       <c r="R67" s="14"/>
     </row>
-    <row r="68" spans="1:20" ht="42" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" ht="28" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
         <v>565</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>668</v>
+        <v>713</v>
       </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
@@ -18740,12 +19068,12 @@
       <c r="Q68" s="14"/>
       <c r="R68" s="14"/>
     </row>
-    <row r="69" spans="1:20" ht="28" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A69" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="B69" s="43" t="s">
-        <v>669</v>
+      <c r="B69" s="49" t="s">
+        <v>714</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
@@ -18769,7 +19097,7 @@
         <v>365</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>747</v>
+        <v>709</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
@@ -18793,7 +19121,7 @@
         <v>366</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>670</v>
+        <v>715</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
@@ -18817,7 +19145,7 @@
         <v>582</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>671</v>
+        <v>716</v>
       </c>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
@@ -18841,7 +19169,7 @@
         <v>582</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>672</v>
+        <v>717</v>
       </c>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
@@ -18996,211 +19324,211 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="14" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="14" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="14" t="s">
-        <v>731</v>
+        <v>693</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>739</v>
+        <v>701</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
-        <v>732</v>
+        <v>694</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>740</v>
+        <v>702</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="14" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
-        <v>733</v>
+        <v>695</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>741</v>
+        <v>703</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="14" t="s">
-        <v>734</v>
+        <v>696</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>742</v>
+        <v>704</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="14" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="14" t="s">
-        <v>735</v>
+        <v>697</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>743</v>
+        <v>705</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="14" t="s">
-        <v>736</v>
+        <v>698</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>744</v>
+        <v>706</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="14" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="14" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="14" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="14" t="s">
-        <v>737</v>
+        <v>699</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>745</v>
+        <v>707</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
-        <v>738</v>
+        <v>700</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>746</v>
+        <v>708</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection insertColumns="0" insertRows="0"/>
   <phoneticPr fontId="34" type="noConversion"/>
-  <conditionalFormatting sqref="A38:A56">
-    <cfRule type="duplicateValues" dxfId="14" priority="495"/>
+  <conditionalFormatting sqref="A39:A57">
+    <cfRule type="duplicateValues" dxfId="13" priority="495"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A80:A81 A83:A88">
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A99:M1048576 N80:XFD1048576 C80:M98">
-    <cfRule type="duplicateValues" dxfId="12" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38:B56">
-    <cfRule type="duplicateValues" dxfId="11" priority="497"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C30">
-    <cfRule type="duplicateValues" dxfId="10" priority="29"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C73">
-    <cfRule type="duplicateValues" dxfId="9" priority="503"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P38:XFD39 Q40:XFD40 P41:XFD46 R47:XFD56">
-    <cfRule type="duplicateValues" dxfId="8" priority="472"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80:A81 A83:A88">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="B39:B57">
+    <cfRule type="duplicateValues" dxfId="10" priority="497"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B80:B88">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C31">
+    <cfRule type="duplicateValues" dxfId="8" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C73">
+    <cfRule type="duplicateValues" dxfId="7" priority="507"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P39:XFD40 Q41:XFD41 P42:XFD47 R48:XFD57">
+    <cfRule type="duplicateValues" dxfId="6" priority="472"/>
   </conditionalFormatting>
   <dataValidations xWindow="367" yWindow="405" count="17">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="One contributer per row, e.g." prompt="Jane, Doe_x000a_Yixin, Wang_x000a_John, H, Smith_x000a_Charles,E,Determan Jr_x000a_Monique,G,van der Wijst_x000a_Mark, Anderson Dumont_x000a_(insert additional rows as needed)_x000a_" sqref="B18:C21" xr:uid="{E3B18FF0-8187-4483-A85F-019FF99D71B4}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="One contributer per row, e.g." prompt="Jane, Doe_x000a_Yixin, Wang_x000a_John, H, Smith_x000a_Charles,E,Determan Jr_x000a_Monique,G,van der Wijst_x000a_Mark, Anderson Dumont_x000a_(insert additional rows as needed)_x000a_" sqref="B18:C22" xr:uid="{E3B18FF0-8187-4483-A85F-019FF99D71B4}"/>
     <dataValidation type="textLength" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Your summary seems too short!" error="Please provide a thorough description of the goals and objectives of this study.  A working abstract from the associated manuscript may be suitable.  Include as much text as necessary." prompt="Please provide a thorough description of the goals and objectives of this study.  A working abstract from the associated manuscript may be suitable.  Include as much text as necessary." sqref="B12:C12" xr:uid="{6DD1BA29-F299-4D8E-AF94-669CA4660371}">
       <formula1>75</formula1>
     </dataValidation>
     <dataValidation type="textLength" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Your design seems too short!" error="From reading the design one should be able to understand the types of samples included in the submission, as well as the experimental conditions and variables under investigation." prompt="From reading the design one should be able to understand the types of SAMPLES included in the submission, as well as the experimental conditions and variables under investigation." sqref="B13:C17" xr:uid="{2912C896-702F-4C65-A59B-F5BEF502C91B}">
       <formula1>75</formula1>
     </dataValidation>
-    <dataValidation type="textLength" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Study title seems too short?" error="Study titles are meant to be informative, such as the title of a manuscript/publication. Can you provide a longer title that is more informative for users?" prompt="Provide a title for this Study. Generally, we recommend the title of an associated manuscript/publication. The title can be updated later, as needed." sqref="B11:C11" xr:uid="{F413C0B7-0301-4079-9A7C-86EB430D5043}">
+    <dataValidation type="textLength" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Study title seems too short?" error="Study titles are meant to be informative, such as the title of a manuscript/publication. Can you provide a longer title that is more informative for users?" prompt="Provide a title for this Study. Generally, we recommend the title of an associated manuscript/publication. The title can be updated later, as needed." sqref="C11" xr:uid="{F413C0B7-0301-4079-9A7C-86EB430D5043}">
       <formula1>50</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="List the name of any processed data files (one per row) that were derived from multiple samples. For instance, bulkRNA-seq tables that include library names as headers, or &quot;merged&quot; peak files." sqref="B22:C22" xr:uid="{38E8CDD9-437B-46E7-BC82-569009D0AD05}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H38:H56" xr:uid="{DD3BF453-67A7-457F-8A50-2AA2F9C643F5}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C63 B22" xr:uid="{1DA8B795-5C89-4577-8836-DB7AEFB725B7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify the library strategy. For example: RNA-seq, scRNA-seq, CITE-seq, Spatial Transcriptomics, ChIP-Seq, CUT&amp;Tag, Bisulfite-seq, ATAC-seq, Hi-C, and so on..." sqref="B63" xr:uid="{3E1B337C-0FAB-46AD-AF75-6E2448C62637}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Identify the organism(s) from which the sequences were derived.  For example:_x000a_Homo sapiens_x000a_Mus musculus_x000a_Arabidopsis thaliana_x000a_Escherichia coli K-12_x000a_Caenorhabditis elegans" sqref="D47:D56 C38:C56" xr:uid="{A870C9A2-F05A-485A-9E21-08C3F86683B5}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the tissue from which this sample was derived. For example:_x000a_Liver_x000a_Breast cancer_x000a_Colorectal cancer_x000a_Liver tumor_x000a_Whole organism_x000a_Mycelium" sqref="D38:D46" xr:uid="{F363101B-E3EB-4921-89A5-DE79B20B09EF}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H39:H40 H43:H44 H47:H49 H52:H54" xr:uid="{47B6B633-8A68-4530-9AD8-BD49CE875996}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I38:I56" xr:uid="{4B61C4DA-D826-4533-9531-93FAAFEF6886}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="List the name of any processed data files (one per row) that were derived from multiple samples. For instance, bulkRNA-seq tables that include library names as headers, or &quot;merged&quot; peak files." sqref="B23:C23" xr:uid="{38E8CDD9-437B-46E7-BC82-569009D0AD05}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H39:H57" xr:uid="{DD3BF453-67A7-457F-8A50-2AA2F9C643F5}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="C64 B23" xr:uid="{1DA8B795-5C89-4577-8836-DB7AEFB725B7}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify the library strategy. For example: RNA-seq, scRNA-seq, CITE-seq, Spatial Transcriptomics, ChIP-Seq, CUT&amp;Tag, Bisulfite-seq, ATAC-seq, Hi-C, and so on..." sqref="B64" xr:uid="{3E1B337C-0FAB-46AD-AF75-6E2448C62637}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Identify the organism(s) from which the sequences were derived.  For example:_x000a_Homo sapiens_x000a_Mus musculus_x000a_Arabidopsis thaliana_x000a_Escherichia coli K-12_x000a_Caenorhabditis elegans" sqref="D48:D57 C39:C57" xr:uid="{A870C9A2-F05A-485A-9E21-08C3F86683B5}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the tissue from which this sample was derived. For example:_x000a_Liver_x000a_Breast cancer_x000a_Colorectal cancer_x000a_Liver tumor_x000a_Whole organism_x000a_Mycelium" sqref="D39:D47" xr:uid="{F363101B-E3EB-4921-89A5-DE79B20B09EF}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Treatment(s) applied to the sample. If no treatments were applied enter 'none'. _x000a_**NOTE: You can insert additional columns before 'molecule' and add more sample descriptions - clinical data, for example**_x000a_" sqref="H40:H41 H44:H45 H48:H50 H53:H55" xr:uid="{47B6B633-8A68-4530-9AD8-BD49CE875996}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I39:I57" xr:uid="{4B61C4DA-D826-4533-9531-93FAAFEF6886}">
       <formula1>"polyA RNA,total RNA, nuclear RNA, cytoplasmic RNA, genomic DNA,protein,other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="J38:J56" xr:uid="{4DF3746A-E025-4F6A-B7CC-339891AC2027}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="J39:J57" xr:uid="{4DF3746A-E025-4F6A-B7CC-339891AC2027}">
       <formula1>"single,paired-end"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell line used, if applicable. For example:_x000a_HeLa_x000a_HEK293_x000a_A549" sqref="E38:E56" xr:uid="{22185DB1-F1B6-4642-9A12-2889E7D560EC}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell type. Examples include:_x000a_PBMCs_x000a_Adipocytes_x000a_neural progenitor cells (NPCs)_x000a_" sqref="F38:F56" xr:uid="{AD947475-09CC-48B9-8265-B9811301F615}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the genotype (if applicable). If not applicable change &quot;genotype&quot; to something else. For example: strain, sex, cultivar, breed, age, developmental stage, etc" sqref="G38:G56" xr:uid="{E4E9BB68-E9AC-40EB-9161-0960CBF212EC}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Each sample title should be unique. _x000a_Use biol/tech rep numbers (when _x000a_applicable) to unique the titles. _x000a_For example:_x000a_Muscle, exercised, 60min, biol rep1_x000a_Muscle, exercised, 60min, biol rep2_x000a_" sqref="B38:C56" xr:uid="{16FCC838-0E0E-48E4-B2AA-D96D65E76279}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell line used, if applicable. For example:_x000a_HeLa_x000a_HEK293_x000a_A549" sqref="E39:E57" xr:uid="{22185DB1-F1B6-4642-9A12-2889E7D560EC}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the cell type. Examples include:_x000a_PBMCs_x000a_Adipocytes_x000a_neural progenitor cells (NPCs)_x000a_" sqref="F39:F57" xr:uid="{AD947475-09CC-48B9-8265-B9811301F615}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="List the genotype (if applicable). If not applicable change &quot;genotype&quot; to something else. For example: strain, sex, cultivar, breed, age, developmental stage, etc" sqref="G39:G57" xr:uid="{E4E9BB68-E9AC-40EB-9161-0960CBF212EC}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="Each sample title should be unique. _x000a_Use biol/tech rep numbers (when _x000a_applicable) to unique the titles. _x000a_For example:_x000a_Muscle, exercised, 60min, biol rep1_x000a_Muscle, exercised, 60min, biol rep2_x000a_" sqref="B39:C57" xr:uid="{16FCC838-0E0E-48E4-B2AA-D96D65E76279}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19213,7 +19541,7 @@
           <x14:formula1>
             <xm:f>'Data validation'!$A$2:$A$58</xm:f>
           </x14:formula1>
-          <xm:sqref>K38:K53 L47:L53 K54:L56</xm:sqref>
+          <xm:sqref>L48:L57</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19228,7 +19556,7 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -19240,32 +19568,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="76" t="s">
         <v>589</v>
       </c>
-      <c r="B1" s="78"/>
+      <c r="B1" s="76"/>
     </row>
     <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="83" t="s">
         <v>594</v>
       </c>
-      <c r="B2" s="76"/>
+      <c r="B2" s="83"/>
     </row>
     <row r="3" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="77"/>
+      <c r="B3" s="84"/>
     </row>
     <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="81" t="s">
         <v>595</v>
       </c>
-      <c r="B4" s="74"/>
+      <c r="B4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82"/>
-      <c r="B5" s="82"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
     </row>
     <row r="6" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -19362,80 +19690,80 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="74"/>
-      <c r="B17" s="74"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="79" t="s">
+      <c r="A18" s="77" t="s">
         <v>266</v>
       </c>
-      <c r="B18" s="80"/>
+      <c r="B18" s="78"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="79" t="s">
         <v>563</v>
       </c>
-      <c r="B19" s="81"/>
+      <c r="B19" s="79"/>
     </row>
     <row r="20" spans="1:6" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="82" t="s">
         <v>591</v>
       </c>
-      <c r="B20" s="75"/>
+      <c r="B20" s="82"/>
       <c r="F20" s="63"/>
     </row>
     <row r="21" spans="1:6" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="82" t="s">
         <v>592</v>
       </c>
-      <c r="B21" s="75"/>
+      <c r="B21" s="82"/>
     </row>
     <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
     </row>
     <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="81"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="74"/>
-      <c r="B25" s="74"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="81"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="74"/>
-      <c r="B26" s="74"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="81"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="74"/>
-      <c r="B27" s="74"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" location="categories" xr:uid="{D6250736-B96D-4C3E-A39D-F5873CF8B173}"/>
@@ -19461,10 +19789,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A6" zoomScale="113" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -19521,269 +19849,463 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
+        <v>620</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>649</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>737</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>651</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>738</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
+        <v>623</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>653</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>739</v>
+      </c>
+      <c r="G11" s="73" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>742</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>740</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="14" t="s">
+        <v>694</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>743</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>741</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>655</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>718</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>657</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>719</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="14" t="s">
+        <v>695</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>744</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>720</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="14" t="s">
+        <v>696</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>745</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>721</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="14" t="s">
+        <v>630</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>659</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>722</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>661</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>723</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="14" t="s">
+        <v>633</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>663</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>724</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="14" t="s">
+        <v>697</v>
+      </c>
+      <c r="B21" s="49" t="s">
+        <v>746</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>725</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="B22" s="49" t="s">
+        <v>747</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>726</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>665</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>727</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="14" t="s">
+        <v>637</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>667</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>728</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="14" t="s">
+        <v>639</v>
+      </c>
+      <c r="B25" s="49" t="s">
+        <v>669</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>729</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="14" t="s">
+        <v>699</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>748</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>730</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="14" t="s">
+        <v>700</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>749</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="14" t="s">
+        <v>619</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>650</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>732</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="14" t="s">
         <v>622</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>673</v>
-      </c>
-      <c r="F9" s="14" t="s">
+      <c r="B29" s="49" t="s">
         <v>652</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>623</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>675</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>653</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>625</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>677</v>
-      </c>
-      <c r="F11" s="14" t="s">
+      <c r="F29" s="14" t="s">
+        <v>733</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="14" t="s">
+        <v>624</v>
+      </c>
+      <c r="B30" s="49" t="s">
         <v>654</v>
       </c>
-      <c r="G11" s="73" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>627</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>679</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>655</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="F30" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>750</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>735</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>751</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>736</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="B33" s="49" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" s="14" t="s">
+        <v>703</v>
+      </c>
+      <c r="B35" s="49" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="14" t="s">
+        <v>704</v>
+      </c>
+      <c r="B36" s="49" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="14" t="s">
         <v>629</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>681</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>656</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="B37" s="49" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" s="14" t="s">
         <v>632</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>683</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>657</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>633</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>685</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>658</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
-        <v>635</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>687</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>659</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>637</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>689</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>660</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
-        <v>639</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>691</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>661</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>641</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>693</v>
-      </c>
-      <c r="F19" s="14" t="s">
+      <c r="B38" s="75" t="s">
         <v>662</v>
       </c>
-      <c r="G19" s="8" t="s">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="14" t="s">
+        <v>634</v>
+      </c>
+      <c r="B39" s="49" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" s="14" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
-        <v>621</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>674</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>663</v>
-      </c>
-      <c r="G20" s="8" t="s">
+      <c r="B40" s="49" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" s="14" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="14" t="s">
-        <v>624</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>676</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>664</v>
-      </c>
-      <c r="G21" s="8" t="s">
+      <c r="B41" s="49" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="B42" s="49" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="B44" s="49" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" s="14" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
-        <v>626</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>628</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
-        <v>630</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
-        <v>631</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
-        <v>634</v>
-      </c>
-      <c r="B26" s="73" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
-        <v>636</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>638</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
-        <v>640</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="14" t="s">
-        <v>642</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>694</v>
+      <c r="B45" s="49" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" s="14" t="s">
+        <v>708</v>
+      </c>
+      <c r="B46" s="75" t="s">
+        <v>757</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A12:A13 A9:A10">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+  <conditionalFormatting sqref="A9:A10 A12:A17">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:A24">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+  <conditionalFormatting sqref="A28:A36">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A31:G1048576 B22:G30 B9:E21 G9:G21">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  <conditionalFormatting sqref="A47:G1048576 C33:G46 G9:G32 C9:E32">
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26732,13 +27254,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="uHeIq0fTY+SkfiG0BUBfkRWN7VsHdDGQfAJwovwYuwp6zuFwWIwuY7JnUgHrIwBV4G25XMH5B7S3rMfU5U3akw==" saltValue="Zz3TVxIHK82bnZabgvGk9Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <conditionalFormatting sqref="A61:E69">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26:Y31">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T26:Y31">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from the drop down menu" sqref="I30:K32" xr:uid="{79D6ECAE-44AD-41AB-84C9-88F44BE0AE81}">

</xml_diff>